<commit_message>
tweaks to the correction system for the questions
</commit_message>
<xml_diff>
--- a/Questions_database1.xlsx
+++ b/Questions_database1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Question-Paper-Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4787B666-45B5-455B-A0CC-4EB620E411AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A3BA36-5A8A-4A9F-BFC6-10ABA0154EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{437AF4A1-82AB-4C11-827D-4A2ECCFE7E6D}"/>
   </bookViews>
@@ -3133,7 +3133,7 @@
     <t>What happened in 1917?</t>
   </si>
   <si>
-    <t>.</t>
+    <t>Question</t>
   </si>
 </sst>
 </file>
@@ -3487,7 +3487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D618A3FA-E129-4AA2-882B-A09F25249852}">
   <dimension ref="A1:A1716"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>